<commit_message>
terminado de reportes en excel
</commit_message>
<xml_diff>
--- a/public/Reporte_de_Entradas.xlsx
+++ b/public/Reporte_de_Entradas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>RESUMEN DE ENTRADAS AL ALMACÉN</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>2023/11/06</t>
+  </si>
+  <si>
+    <t>2023/11/07</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -119,7 +122,7 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -207,6 +210,41 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2047875" cy="381000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="nombre_master_pizza" descr="nombre_master_pizza"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,10 +537,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A52" sqref="A52:F52"/>
+      <selection activeCell="A53" sqref="A53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,6 +553,9 @@
     <col min="6" max="6" width="20" customWidth="true" style="0"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1"/>
+    </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -1486,29 +1527,49 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="3">
+        <v>48</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6">
-        <f>SUM(D5:D52)</f>
-        <v>7275.5</v>
-      </c>
-      <c r="E52" s="6">
-        <f>SUM(E5:E52)</f>
+      <c r="C52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F52" s="4">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6">
+        <f>SUM(D5:D53)</f>
+        <v>7305.5</v>
+      </c>
+      <c r="E53" s="6">
+        <f>SUM(E5:E53)</f>
         <v>483.405</v>
       </c>
-      <c r="F52" s="6">
-        <f>SUM(F5:F52)</f>
-        <v>6792.095</v>
+      <c r="F53" s="6">
+        <f>SUM(F5:F53)</f>
+        <v>6822.095</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A53:C53"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,6 +1582,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>